<commit_message>
updated results after minor tweak to text multiplier method
</commit_message>
<xml_diff>
--- a/perf-table.xlsx
+++ b/perf-table.xlsx
@@ -424,16 +424,16 @@
                   <c:v>15.000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5578.000000</c:v>
+                  <c:v>5754.000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11428.000000</c:v>
+                  <c:v>11914.000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24641.000000</c:v>
+                  <c:v>25130.000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28197.000000</c:v>
+                  <c:v>28766.000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -518,19 +518,19 @@
               <c:numCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>13.000000</c:v>
+                  <c:v>15.000000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2177.000000</c:v>
+                  <c:v>2226.000000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4398.000000</c:v>
+                  <c:v>4435.000000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8008.000000</c:v>
+                  <c:v>8084.000000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9947.000000</c:v>
+                  <c:v>9900.000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1820,7 +1820,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="6">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1830,10 +1830,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="8">
-        <v>5578</v>
+        <v>5754</v>
       </c>
       <c r="C5" s="9">
-        <v>2177</v>
+        <v>2226</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -1843,10 +1843,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="10">
-        <v>11428</v>
+        <v>11914</v>
       </c>
       <c r="C6" s="11">
-        <v>4398</v>
+        <v>4435</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -1856,10 +1856,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="8">
-        <v>24641</v>
+        <v>25130</v>
       </c>
       <c r="C7" s="9">
-        <v>8008</v>
+        <v>8084</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -1869,10 +1869,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="10">
-        <v>28197</v>
+        <v>28766</v>
       </c>
       <c r="C8" s="11">
-        <v>9947</v>
+        <v>9900</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>

</xml_diff>